<commit_message>
Making edits per Dr. Thomas's comments
</commit_message>
<xml_diff>
--- a/Project Planning/Project Plan.xlsx
+++ b/Project Planning/Project Plan.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20904"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20325"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://msoe365-my.sharepoint.com/personal/windorffj_msoe_edu/Documents/Senior Design/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\larsonma\Documents\SeniorDesign\Project Planning\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="25" documentId="8_{DFFEE05D-782E-4655-8600-ACF64D939964}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{059E9E58-C360-4101-B1E6-E76907F2A2C6}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{6F7BFD90-6A92-498D-8DB3-E770464E8F21}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12225" xr2:uid="{C981FB62-2ABF-4AA1-9EAB-0DCB3DE17D6E}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12228" xr2:uid="{C981FB62-2ABF-4AA1-9EAB-0DCB3DE17D6E}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="40">
   <si>
     <t>Development Process</t>
   </si>
@@ -102,41 +102,69 @@
     <t>Identify and order prototyping devices</t>
   </si>
   <si>
-    <t>Technology and Concept Investigation report done </t>
-  </si>
-  <si>
-    <t>Finish system repuirements and interface design</t>
-  </si>
-  <si>
     <t>Begin Prototyping Hardware. System requirements specification done</t>
   </si>
   <si>
-    <t>Complete cycle report</t>
-  </si>
-  <si>
-    <t>Finish Prototyping</t>
-  </si>
-  <si>
-    <t>Design Deliverables Done</t>
-  </si>
-  <si>
-    <t>Finish integration testing</t>
-  </si>
-  <si>
-    <t>Final Presentation Prepared</t>
-  </si>
-  <si>
     <t>Tech and concept investigation</t>
   </si>
   <si>
-    <t>Prototyping (~7 weeks)</t>
+    <t>Technology and Concept Investigation report done 
+Date: 10/3/18</t>
+  </si>
+  <si>
+    <t>Finish system repuirements and interface design
+Date: 10/19/18</t>
+  </si>
+  <si>
+    <t>Complete cycle report
+Date: 11/9/18</t>
+  </si>
+  <si>
+    <t>Finish Prototyping
+Date: 12/7/18</t>
+  </si>
+  <si>
+    <t>Design Deliverables Done
+2/1/19</t>
+  </si>
+  <si>
+    <t>Finish integration testing
+Date: 3/15/19</t>
+  </si>
+  <si>
+    <t>Final Presentation Prepared
+Date: 4/26/18</t>
+  </si>
+  <si>
+    <t>Practive Final Prenstation
+Make Final revisions to documents</t>
+  </si>
+  <si>
+    <t>Work on Final Presentation
+Finalize all doucmentation
+Finalize product presentation</t>
+  </si>
+  <si>
+    <t>System and Integration Testing</t>
+  </si>
+  <si>
+    <t>Design Work
+Iterative Testing</t>
+  </si>
+  <si>
+    <t>System Requirments
+Interface Design</t>
+  </si>
+  <si>
+    <t>Prototyping (~7 weeks)
+Design Planning</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -306,7 +334,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -338,28 +366,31 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -678,39 +709,41 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BA51A460-2896-4291-8BB7-539F89C11202}">
   <dimension ref="A2:AF14"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0" xr3:uid="{807A558E-4900-5DB5-BACC-B8507F184E2D}">
-      <selection activeCell="T13" sqref="T13"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="D20" sqref="D20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="14.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="15.42578125" style="1" customWidth="1"/>
-    <col min="3" max="3" width="14.140625" style="1" customWidth="1"/>
-    <col min="4" max="4" width="9.140625" style="1"/>
+    <col min="1" max="1" width="14.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.44140625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="14.109375" style="1" customWidth="1"/>
+    <col min="4" max="4" width="9.109375" style="1"/>
     <col min="5" max="5" width="16" style="1" customWidth="1"/>
-    <col min="6" max="6" width="9.140625" style="1"/>
-    <col min="7" max="7" width="14.28515625" style="1" customWidth="1"/>
-    <col min="8" max="8" width="15.5703125" style="1" customWidth="1"/>
-    <col min="9" max="9" width="9.140625" style="1"/>
+    <col min="6" max="6" width="9.109375" style="1"/>
+    <col min="7" max="7" width="14.33203125" style="1" customWidth="1"/>
+    <col min="8" max="8" width="15.5546875" style="1" customWidth="1"/>
+    <col min="9" max="9" width="9.109375" style="1"/>
     <col min="10" max="10" width="14" style="1" customWidth="1"/>
-    <col min="11" max="12" width="9.140625" style="1"/>
-    <col min="13" max="13" width="16.85546875" style="1" customWidth="1"/>
-    <col min="14" max="23" width="9.140625" style="1"/>
+    <col min="11" max="12" width="9.109375" style="1"/>
+    <col min="13" max="13" width="16.88671875" style="1" customWidth="1"/>
+    <col min="14" max="23" width="9.109375" style="1"/>
     <col min="24" max="24" width="14" style="1" customWidth="1"/>
-    <col min="25" max="16384" width="9.140625" style="1"/>
+    <col min="25" max="28" width="9.109375" style="1"/>
+    <col min="29" max="29" width="12.33203125" style="1" customWidth="1"/>
+    <col min="30" max="16384" width="9.109375" style="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:32" ht="23.25">
-      <c r="A2" s="11" t="s">
+    <row r="2" spans="1:32" ht="23.4" x14ac:dyDescent="0.3">
+      <c r="A2" s="17" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="11"/>
-      <c r="C2" s="11"/>
-      <c r="D2" s="11"/>
-      <c r="E2" s="11"/>
+      <c r="B2" s="17"/>
+      <c r="C2" s="17"/>
+      <c r="D2" s="17"/>
+      <c r="E2" s="17"/>
     </row>
-    <row r="3" spans="1:32">
+    <row r="3" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A3" s="12" t="s">
         <v>1</v>
       </c>
@@ -719,7 +752,7 @@
       <c r="D3" s="12"/>
       <c r="E3" s="12"/>
     </row>
-    <row r="4" spans="1:32">
+    <row r="4" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A4" s="12" t="s">
         <v>2</v>
       </c>
@@ -728,7 +761,7 @@
       <c r="D4" s="12"/>
       <c r="E4" s="12"/>
     </row>
-    <row r="5" spans="1:32">
+    <row r="5" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A5" s="12" t="s">
         <v>3</v>
       </c>
@@ -737,7 +770,7 @@
       <c r="D5" s="12"/>
       <c r="E5" s="12"/>
     </row>
-    <row r="6" spans="1:32">
+    <row r="6" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A6" s="12" t="s">
         <v>4</v>
       </c>
@@ -746,117 +779,117 @@
       <c r="D6" s="12"/>
       <c r="E6" s="12"/>
     </row>
-    <row r="8" spans="1:32" ht="15" customHeight="1">
-      <c r="A8" s="13" t="s">
+    <row r="8" spans="1:32" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="18" t="s">
         <v>5</v>
       </c>
-      <c r="B8" s="13"/>
-      <c r="C8" s="13"/>
-      <c r="D8" s="13"/>
-      <c r="E8" s="13"/>
-      <c r="F8" s="13"/>
-      <c r="G8" s="13"/>
-      <c r="H8" s="13"/>
-      <c r="I8" s="13"/>
-      <c r="J8" s="13"/>
-      <c r="K8" s="13"/>
-      <c r="L8" s="13"/>
-      <c r="M8" s="13"/>
-      <c r="N8" s="13"/>
-      <c r="O8" s="13"/>
-      <c r="P8" s="13"/>
-      <c r="Q8" s="13"/>
-      <c r="R8" s="13"/>
-      <c r="S8" s="13"/>
-      <c r="T8" s="13"/>
-      <c r="U8" s="13"/>
-      <c r="V8" s="13"/>
-      <c r="W8" s="13"/>
-      <c r="X8" s="13"/>
-      <c r="Y8" s="13"/>
-      <c r="Z8" s="13"/>
-      <c r="AA8" s="13"/>
-      <c r="AB8" s="13"/>
-      <c r="AC8" s="13"/>
-      <c r="AD8" s="13"/>
-      <c r="AE8" s="13"/>
-      <c r="AF8" s="13"/>
+      <c r="B8" s="18"/>
+      <c r="C8" s="18"/>
+      <c r="D8" s="18"/>
+      <c r="E8" s="18"/>
+      <c r="F8" s="18"/>
+      <c r="G8" s="18"/>
+      <c r="H8" s="18"/>
+      <c r="I8" s="18"/>
+      <c r="J8" s="18"/>
+      <c r="K8" s="18"/>
+      <c r="L8" s="18"/>
+      <c r="M8" s="18"/>
+      <c r="N8" s="18"/>
+      <c r="O8" s="18"/>
+      <c r="P8" s="18"/>
+      <c r="Q8" s="18"/>
+      <c r="R8" s="18"/>
+      <c r="S8" s="18"/>
+      <c r="T8" s="18"/>
+      <c r="U8" s="18"/>
+      <c r="V8" s="18"/>
+      <c r="W8" s="18"/>
+      <c r="X8" s="18"/>
+      <c r="Y8" s="18"/>
+      <c r="Z8" s="18"/>
+      <c r="AA8" s="18"/>
+      <c r="AB8" s="18"/>
+      <c r="AC8" s="18"/>
+      <c r="AD8" s="18"/>
+      <c r="AE8" s="18"/>
+      <c r="AF8" s="18"/>
     </row>
-    <row r="9" spans="1:32" ht="15" customHeight="1">
-      <c r="A9" s="13"/>
-      <c r="B9" s="13"/>
-      <c r="C9" s="13"/>
-      <c r="D9" s="13"/>
-      <c r="E9" s="13"/>
-      <c r="F9" s="13"/>
-      <c r="G9" s="13"/>
-      <c r="H9" s="13"/>
-      <c r="I9" s="13"/>
-      <c r="J9" s="13"/>
-      <c r="K9" s="13"/>
-      <c r="L9" s="13"/>
-      <c r="M9" s="13"/>
-      <c r="N9" s="13"/>
-      <c r="O9" s="13"/>
-      <c r="P9" s="13"/>
-      <c r="Q9" s="13"/>
-      <c r="R9" s="13"/>
-      <c r="S9" s="13"/>
-      <c r="T9" s="13"/>
-      <c r="U9" s="13"/>
-      <c r="V9" s="13"/>
-      <c r="W9" s="13"/>
-      <c r="X9" s="13"/>
-      <c r="Y9" s="13"/>
-      <c r="Z9" s="13"/>
-      <c r="AA9" s="13"/>
-      <c r="AB9" s="13"/>
-      <c r="AC9" s="13"/>
-      <c r="AD9" s="13"/>
-      <c r="AE9" s="13"/>
-      <c r="AF9" s="13"/>
+    <row r="9" spans="1:32" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="18"/>
+      <c r="B9" s="18"/>
+      <c r="C9" s="18"/>
+      <c r="D9" s="18"/>
+      <c r="E9" s="18"/>
+      <c r="F9" s="18"/>
+      <c r="G9" s="18"/>
+      <c r="H9" s="18"/>
+      <c r="I9" s="18"/>
+      <c r="J9" s="18"/>
+      <c r="K9" s="18"/>
+      <c r="L9" s="18"/>
+      <c r="M9" s="18"/>
+      <c r="N9" s="18"/>
+      <c r="O9" s="18"/>
+      <c r="P9" s="18"/>
+      <c r="Q9" s="18"/>
+      <c r="R9" s="18"/>
+      <c r="S9" s="18"/>
+      <c r="T9" s="18"/>
+      <c r="U9" s="18"/>
+      <c r="V9" s="18"/>
+      <c r="W9" s="18"/>
+      <c r="X9" s="18"/>
+      <c r="Y9" s="18"/>
+      <c r="Z9" s="18"/>
+      <c r="AA9" s="18"/>
+      <c r="AB9" s="18"/>
+      <c r="AC9" s="18"/>
+      <c r="AD9" s="18"/>
+      <c r="AE9" s="18"/>
+      <c r="AF9" s="18"/>
     </row>
-    <row r="10" spans="1:32" ht="15" customHeight="1">
-      <c r="A10" s="17" t="s">
+    <row r="10" spans="1:32" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="15" t="s">
         <v>6</v>
       </c>
-      <c r="B10" s="17"/>
-      <c r="C10" s="17"/>
-      <c r="D10" s="17"/>
-      <c r="E10" s="17"/>
-      <c r="F10" s="17"/>
-      <c r="G10" s="17"/>
-      <c r="H10" s="17"/>
-      <c r="I10" s="17"/>
-      <c r="J10" s="17"/>
+      <c r="B10" s="15"/>
+      <c r="C10" s="15"/>
+      <c r="D10" s="15"/>
+      <c r="E10" s="15"/>
+      <c r="F10" s="15"/>
+      <c r="G10" s="15"/>
+      <c r="H10" s="15"/>
+      <c r="I10" s="15"/>
+      <c r="J10" s="15"/>
       <c r="K10" s="2"/>
-      <c r="L10" s="18" t="s">
+      <c r="L10" s="16" t="s">
         <v>7</v>
       </c>
-      <c r="M10" s="18"/>
-      <c r="N10" s="18"/>
-      <c r="O10" s="18"/>
-      <c r="P10" s="18"/>
-      <c r="Q10" s="18"/>
-      <c r="R10" s="18"/>
-      <c r="S10" s="18"/>
-      <c r="T10" s="18"/>
-      <c r="U10" s="18"/>
+      <c r="M10" s="16"/>
+      <c r="N10" s="16"/>
+      <c r="O10" s="16"/>
+      <c r="P10" s="16"/>
+      <c r="Q10" s="16"/>
+      <c r="R10" s="16"/>
+      <c r="S10" s="16"/>
+      <c r="T10" s="16"/>
+      <c r="U10" s="16"/>
       <c r="V10" s="2"/>
-      <c r="W10" s="14" t="s">
+      <c r="W10" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="X10" s="14"/>
-      <c r="Y10" s="14"/>
-      <c r="Z10" s="14"/>
-      <c r="AA10" s="14"/>
-      <c r="AB10" s="14"/>
-      <c r="AC10" s="14"/>
-      <c r="AD10" s="14"/>
-      <c r="AE10" s="14"/>
-      <c r="AF10" s="14"/>
+      <c r="X10" s="11"/>
+      <c r="Y10" s="11"/>
+      <c r="Z10" s="11"/>
+      <c r="AA10" s="11"/>
+      <c r="AB10" s="11"/>
+      <c r="AC10" s="11"/>
+      <c r="AD10" s="11"/>
+      <c r="AE10" s="11"/>
+      <c r="AF10" s="11"/>
     </row>
-    <row r="11" spans="1:32" ht="15" customHeight="1">
+    <row r="11" spans="1:32" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="12" t="s">
         <v>9</v>
       </c>
@@ -896,7 +929,7 @@
       <c r="AE11" s="12"/>
       <c r="AF11" s="12"/>
     </row>
-    <row r="12" spans="1:32">
+    <row r="12" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A12" s="4" t="s">
         <v>12</v>
       </c>
@@ -990,7 +1023,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="13" spans="1:32" ht="105">
+    <row r="13" spans="1:32" ht="72" x14ac:dyDescent="0.3">
       <c r="A13" s="3" t="s">
         <v>22</v>
       </c>
@@ -1002,22 +1035,22 @@
       </c>
       <c r="D13" s="9"/>
       <c r="E13" s="9" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="F13" s="9"/>
       <c r="G13" s="7" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="H13" s="1" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="I13" s="10"/>
       <c r="J13" s="10" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="K13" s="2"/>
       <c r="M13" s="6" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="N13" s="6"/>
       <c r="O13" s="6"/>
@@ -1025,74 +1058,93 @@
       <c r="Q13" s="6"/>
       <c r="R13" s="6"/>
       <c r="S13" s="6" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="T13" s="6"/>
       <c r="U13" s="6"/>
       <c r="V13" s="2"/>
       <c r="X13" s="6" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="Y13" s="6"/>
       <c r="Z13" s="6"/>
       <c r="AA13" s="6"/>
       <c r="AB13" s="6"/>
       <c r="AC13" s="6" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="AD13" s="6"/>
       <c r="AE13" s="6"/>
       <c r="AF13" s="6"/>
     </row>
-    <row r="14" spans="1:32" ht="45" customHeight="1">
-      <c r="B14" s="15" t="s">
-        <v>33</v>
+    <row r="14" spans="1:32" ht="45" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B14" s="13" t="s">
+        <v>26</v>
       </c>
       <c r="C14" s="12"/>
       <c r="D14" s="12"/>
-      <c r="E14" s="16"/>
-      <c r="H14" s="15" t="s">
+      <c r="E14" s="14"/>
+      <c r="F14" s="13" t="s">
+        <v>38</v>
+      </c>
+      <c r="G14" s="14"/>
+      <c r="H14" s="13" t="s">
+        <v>39</v>
+      </c>
+      <c r="I14" s="19"/>
+      <c r="J14" s="19"/>
+      <c r="K14" s="19"/>
+      <c r="L14" s="19"/>
+      <c r="M14" s="14"/>
+      <c r="N14" s="13" t="s">
+        <v>37</v>
+      </c>
+      <c r="O14" s="19"/>
+      <c r="P14" s="19"/>
+      <c r="Q14" s="19"/>
+      <c r="R14" s="19"/>
+      <c r="S14" s="14"/>
+      <c r="T14" s="13" t="s">
+        <v>36</v>
+      </c>
+      <c r="U14" s="19"/>
+      <c r="V14" s="19"/>
+      <c r="W14" s="19"/>
+      <c r="X14" s="14"/>
+      <c r="Y14" s="13" t="s">
+        <v>35</v>
+      </c>
+      <c r="Z14" s="19"/>
+      <c r="AA14" s="19"/>
+      <c r="AB14" s="14"/>
+      <c r="AC14" s="13" t="s">
         <v>34</v>
       </c>
-      <c r="I14" s="12"/>
-      <c r="J14" s="12"/>
-      <c r="K14" s="2"/>
-      <c r="M14" s="6"/>
-      <c r="N14" s="6"/>
-      <c r="O14" s="6"/>
-      <c r="P14" s="6"/>
-      <c r="Q14" s="6"/>
-      <c r="R14" s="6"/>
-      <c r="S14" s="6"/>
-      <c r="T14" s="6"/>
-      <c r="U14" s="6"/>
-      <c r="V14" s="2"/>
-      <c r="X14" s="6"/>
-      <c r="Y14" s="6"/>
-      <c r="Z14" s="6"/>
-      <c r="AA14" s="6"/>
-      <c r="AB14" s="6"/>
-      <c r="AC14" s="6"/>
-      <c r="AD14" s="6"/>
-      <c r="AE14" s="6"/>
-      <c r="AF14" s="6"/>
+      <c r="AD14" s="19"/>
+      <c r="AE14" s="19"/>
+      <c r="AF14" s="19"/>
     </row>
   </sheetData>
-  <mergeCells count="14">
-    <mergeCell ref="W10:AF10"/>
-    <mergeCell ref="W11:AF11"/>
-    <mergeCell ref="B14:E14"/>
-    <mergeCell ref="H14:J14"/>
-    <mergeCell ref="A11:J11"/>
-    <mergeCell ref="A10:J10"/>
-    <mergeCell ref="L10:U10"/>
-    <mergeCell ref="L11:U11"/>
+  <mergeCells count="19">
     <mergeCell ref="A2:E2"/>
     <mergeCell ref="A3:E3"/>
     <mergeCell ref="A4:E4"/>
     <mergeCell ref="A8:AF9"/>
     <mergeCell ref="A5:E5"/>
     <mergeCell ref="A6:E6"/>
+    <mergeCell ref="W10:AF10"/>
+    <mergeCell ref="W11:AF11"/>
+    <mergeCell ref="B14:E14"/>
+    <mergeCell ref="A11:J11"/>
+    <mergeCell ref="A10:J10"/>
+    <mergeCell ref="L10:U10"/>
+    <mergeCell ref="L11:U11"/>
+    <mergeCell ref="AC14:AF14"/>
+    <mergeCell ref="Y14:AB14"/>
+    <mergeCell ref="T14:X14"/>
+    <mergeCell ref="N14:S14"/>
+    <mergeCell ref="H14:M14"/>
+    <mergeCell ref="F14:G14"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>